<commit_message>
still has errors with exceeding max guests
</commit_message>
<xml_diff>
--- a/Running Dinner eerste oplossing 2022.xlsx
+++ b/Running Dinner eerste oplossing 2022.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stichtingfontys-my.sharepoint.com/personal/507827_student_fontys_nl/Documents/Documenten/Jaar2/OR5_RunningDinner/OR5_project/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_FFC65FC07081A9CE68170B4D9B8EF459746A0BB6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1C162E0-7D05-4BBF-9CCB-EA3013D863FE}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -541,8 +547,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -601,17 +607,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -649,7 +663,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -683,6 +697,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -717,9 +732,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -892,14 +908,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -922,7 +943,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -942,7 +963,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -968,7 +989,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -994,7 +1015,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1020,7 +1041,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1046,7 +1067,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1072,7 +1093,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1098,7 +1119,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1118,7 +1139,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1138,7 +1159,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1164,7 +1185,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1190,7 +1211,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1216,7 +1237,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1242,7 +1263,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1268,7 +1289,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1294,7 +1315,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1320,7 +1341,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1346,7 +1367,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1372,7 +1393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1392,7 +1413,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1418,7 +1439,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1438,7 +1459,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1464,7 +1485,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1490,7 +1511,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1516,7 +1537,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1542,7 +1563,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1568,7 +1589,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1594,7 +1615,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1620,7 +1641,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1646,7 +1667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1672,7 +1693,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1698,7 +1719,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1724,7 +1745,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1750,7 +1771,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1770,7 +1791,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1796,7 +1817,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1822,7 +1843,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1848,7 +1869,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1874,7 +1895,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1900,7 +1921,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1926,7 +1947,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1946,7 +1967,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1972,7 +1993,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1998,7 +2019,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2024,7 +2045,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2050,7 +2071,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2076,7 +2097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2102,7 +2123,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2128,7 +2149,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2148,7 +2169,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2174,7 +2195,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2200,7 +2221,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2220,7 +2241,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2246,7 +2267,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2272,7 +2293,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2298,7 +2319,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2324,7 +2345,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2350,7 +2371,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2376,7 +2397,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2396,7 +2417,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2422,7 +2443,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2448,7 +2469,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2474,7 +2495,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2500,7 +2521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2526,7 +2547,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2552,7 +2573,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2578,7 +2599,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2604,7 +2625,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2630,7 +2651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2656,7 +2677,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2682,7 +2703,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2708,7 +2729,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2734,7 +2755,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2760,7 +2781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2786,7 +2807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2812,7 +2833,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2838,7 +2859,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2864,7 +2885,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -2890,7 +2911,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2916,7 +2937,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2942,7 +2963,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2968,7 +2989,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2988,7 +3009,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -3014,7 +3035,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -3040,7 +3061,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -3066,7 +3087,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -3092,7 +3113,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -3118,7 +3139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -3144,7 +3165,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -3170,7 +3191,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -3196,7 +3217,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -3216,7 +3237,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -3242,7 +3263,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -3268,7 +3289,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -3288,7 +3309,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -3308,7 +3329,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -3334,7 +3355,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -3360,7 +3381,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -3386,7 +3407,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -3412,7 +3433,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -3438,7 +3459,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -3464,7 +3485,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -3490,7 +3511,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -3516,7 +3537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -3542,7 +3563,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -3568,7 +3589,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -3594,7 +3615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -3620,7 +3641,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -3646,7 +3667,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -3672,7 +3693,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>109</v>
       </c>

</xml_diff>